<commit_message>
up truoc khi di hoc
</commit_message>
<xml_diff>
--- a/dbb.xlsx
+++ b/dbb.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT\ki4\PRJ\AssG10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT\ki4\PRJ\AssG10\PRJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>sinhVien</t>
   </si>
@@ -307,6 +307,41 @@
         <scheme val="minor"/>
       </rPr>
       <t>anhSinhVien</t>
+    </r>
+  </si>
+  <si>
+    <t>bqt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>banquantriId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,  firstName, lastName, gioiTinh, ngaySinh, soDienThoai, gmail, diaChi, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>idCoSo , giangVienId,</t>
     </r>
   </si>
 </sst>
@@ -652,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,6 +772,14 @@
         <v>16</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
co ban cua bqt
</commit_message>
<xml_diff>
--- a/dbb.xlsx
+++ b/dbb.xlsx
@@ -180,6 +180,147 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>quanTriId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, firstName, lastName, gioiTinh, ngaySinh, soDienThoai, gmail, diaChi, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>idCoSo, taiKhoanId</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>phuHuynhId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,  firstName, lastName, gioiTinh, ngaySinh, soDienThoai, gmail, diaChi, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>idCoSo , sinhVienId, taiKhoanId</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sinhVienId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, firstName, lastName, gioiTinh, ngaySinh, soDienThoai, gmail, diaChi, batDauTu, ketThucNgay,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> idChuyenNganh, idCoSo, trangThaiId, taiKhoanId, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>anhSinhVien</t>
+    </r>
+  </si>
+  <si>
+    <t>canBo</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>canBoId,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  firstName, lastName, gioiTinh, ngaySinh, soDienThoai, gmail, diaChi, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>idCoSo , taiKhoanId</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>giangVienId,</t>
     </r>
     <r>
@@ -190,148 +331,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">  firstName, lastName, gioiTinh, ngaySinh, soDienThoai, gmail, diaChi, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>idCoSo , taiKhoanId</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>quanTriId</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, firstName, lastName, gioiTinh, ngaySinh, soDienThoai, gmail, diaChi, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>idCoSo, taiKhoanId</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>phuHuynhId</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">,  firstName, lastName, gioiTinh, ngaySinh, soDienThoai, gmail, diaChi, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>idCoSo , sinhVienId, taiKhoanId</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>sinhVienId</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, firstName, lastName, gioiTinh, ngaySinh, soDienThoai, gmail, diaChi, batDauTu, ketThucNgay,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> idChuyenNganh, idCoSo, trangThaiId, taiKhoanId, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>anhSinhVien</t>
-    </r>
-  </si>
-  <si>
-    <t>canBo</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>canBoId,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  firstName, lastName, gioiTinh, ngaySinh, soDienThoai, gmail, diaChi, </t>
+      <t xml:space="preserve">  firstName, lastName, gioiTinh, ngaySinh, batDauTu, ketThucNgay, soDienThoai, gmail, diaChi, </t>
     </r>
     <r>
       <rPr>
@@ -690,7 +690,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +745,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -753,7 +753,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -761,7 +761,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -769,15 +769,15 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>